<commit_message>
Verificacoes para evitar repeticao de dados
</commit_message>
<xml_diff>
--- a/Infosis Banco/worksheet.xlsx
+++ b/Infosis Banco/worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Infosis Banco\Infosis Banco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E70C6D-6A9D-460A-8D05-FA6BC4176A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730ECEA0-735E-4DD9-9082-B2426BB28CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>PORCENTAGEM_TB</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>RUA AMILTON</t>
+  </si>
+  <si>
+    <t>DBA</t>
+  </si>
+  <si>
+    <t>JUNIOR</t>
   </si>
 </sst>
 </file>
@@ -513,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +761,7 @@
         <v>17</v>
       </c>
       <c r="F5">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="G5">
         <v>50</v>
@@ -777,15 +783,66 @@
       </c>
       <c r="M5">
         <f>F5*50%</f>
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="N5" s="5">
-        <v>44906</v>
+        <v>44899</v>
       </c>
       <c r="O5" s="6">
         <v>50</v>
       </c>
       <c r="P5" s="5">
+        <v>44905</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>999238821</v>
+      </c>
+      <c r="L6">
+        <v>2324981042</v>
+      </c>
+      <c r="M6">
+        <f>F6*50%</f>
+        <v>50</v>
+      </c>
+      <c r="N6" s="5">
+        <v>44899</v>
+      </c>
+      <c r="O6" s="6">
+        <v>50</v>
+      </c>
+      <c r="P6" s="5">
         <v>44905</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionandos as propriedades do endereco a planilha
</commit_message>
<xml_diff>
--- a/Infosis Banco/worksheet.xlsx
+++ b/Infosis Banco/worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Infosis Banco\Infosis Banco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730ECEA0-735E-4DD9-9082-B2426BB28CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D817218-6420-46EB-8640-D2539B2EC7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
   <si>
     <t>PORCENTAGEM_TB</t>
   </si>
@@ -62,9 +62,6 @@
     <t>NOME</t>
   </si>
   <si>
-    <t>ENDERECO</t>
-  </si>
-  <si>
     <t>CPF</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>PEDRO</t>
   </si>
   <si>
-    <t>RUA CARIJO</t>
-  </si>
-  <si>
     <t>DATA_DP</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>JOÃO</t>
   </si>
   <si>
-    <t>RUA CARLOS</t>
-  </si>
-  <si>
     <t>SOBRENOME</t>
   </si>
   <si>
@@ -159,6 +150,54 @@
   </si>
   <si>
     <t>JUNIOR</t>
+  </si>
+  <si>
+    <t>RUA</t>
+  </si>
+  <si>
+    <t>BAIRRO</t>
+  </si>
+  <si>
+    <t>CIDADE</t>
+  </si>
+  <si>
+    <t>NUMERO</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>UF</t>
+  </si>
+  <si>
+    <t>RUA PEDRO</t>
+  </si>
+  <si>
+    <t>ARARA</t>
+  </si>
+  <si>
+    <t>VITORIA</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>RUA JOAO</t>
+  </si>
+  <si>
+    <t>ONÇA</t>
+  </si>
+  <si>
+    <t>COBRA</t>
+  </si>
+  <si>
+    <t>RUA SANCHEZ</t>
+  </si>
+  <si>
+    <t>GATO</t>
+  </si>
+  <si>
+    <t>TATU</t>
   </si>
 </sst>
 </file>
@@ -519,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,16 +571,17 @@
     <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="7" width="12.140625" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" customWidth="1"/>
+    <col min="19" max="19" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -567,16 +607,16 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>
@@ -585,27 +625,42 @@
         <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
       </c>
       <c r="F2">
         <v>100</v>
@@ -614,49 +669,64 @@
         <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
+        <v>30</v>
+      </c>
+      <c r="J2">
+        <v>992345232</v>
       </c>
       <c r="K2">
-        <v>992345232</v>
+        <v>23342312312</v>
       </c>
       <c r="L2">
-        <v>23342312312</v>
-      </c>
-      <c r="M2">
         <f>F2*50%</f>
         <v>50</v>
       </c>
-      <c r="N2" s="5">
+      <c r="M2" s="5">
         <v>44899</v>
       </c>
-      <c r="O2">
-        <v>50</v>
-      </c>
-      <c r="P2" s="5">
+      <c r="N2">
+        <v>50</v>
+      </c>
+      <c r="O2" s="5">
         <v>44898</v>
       </c>
+      <c r="P2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S2">
+        <v>1010</v>
+      </c>
+      <c r="T2">
+        <v>29040230</v>
+      </c>
+      <c r="U2" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
       </c>
       <c r="F3">
         <v>400</v>
@@ -665,49 +735,64 @@
         <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
+        <v>31</v>
+      </c>
+      <c r="J3">
+        <v>994827392</v>
       </c>
       <c r="K3">
-        <v>994827392</v>
+        <v>19492784921</v>
       </c>
       <c r="L3">
-        <v>19492784921</v>
-      </c>
-      <c r="M3">
         <f>F3*50%</f>
         <v>200</v>
       </c>
-      <c r="N3" s="5">
+      <c r="M3" s="5">
         <v>44904</v>
       </c>
-      <c r="O3">
+      <c r="N3">
         <v>75</v>
       </c>
-      <c r="P3" s="5">
+      <c r="O3" s="5">
         <v>44903</v>
       </c>
+      <c r="P3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" t="s">
+        <v>46</v>
+      </c>
+      <c r="S3">
+        <v>2932</v>
+      </c>
+      <c r="T3">
+        <v>29060392</v>
+      </c>
+      <c r="U3" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>8</v>
       </c>
       <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
         <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
       </c>
       <c r="F4">
         <v>300</v>
@@ -716,49 +801,64 @@
         <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="J4">
+        <v>999248293</v>
       </c>
       <c r="K4">
-        <v>999248293</v>
-      </c>
-      <c r="L4">
         <v>19482392392</v>
       </c>
-      <c r="M4" s="6">
+      <c r="L4" s="6">
         <f>F4*50%</f>
         <v>150</v>
       </c>
-      <c r="N4" s="5">
+      <c r="M4" s="5">
         <v>44905</v>
       </c>
-      <c r="O4" s="6">
-        <v>50</v>
-      </c>
-      <c r="P4" s="5">
+      <c r="N4" s="6">
+        <v>50</v>
+      </c>
+      <c r="O4" s="5">
         <v>44904</v>
       </c>
+      <c r="P4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S4">
+        <v>2832</v>
+      </c>
+      <c r="T4">
+        <v>29040382</v>
+      </c>
+      <c r="U4" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>8</v>
       </c>
       <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
       </c>
       <c r="F5">
         <v>250</v>
@@ -767,49 +867,64 @@
         <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="J5">
+        <v>923929393</v>
       </c>
       <c r="K5">
-        <v>923929393</v>
+        <v>29329329392</v>
       </c>
       <c r="L5">
-        <v>29329329392</v>
-      </c>
-      <c r="M5">
         <f>F5*50%</f>
         <v>125</v>
       </c>
-      <c r="N5" s="5">
+      <c r="M5" s="5">
         <v>44899</v>
       </c>
-      <c r="O5" s="6">
-        <v>50</v>
-      </c>
-      <c r="P5" s="5">
+      <c r="N5" s="6">
+        <v>50</v>
+      </c>
+      <c r="O5" s="5">
         <v>44905</v>
       </c>
+      <c r="P5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R5" t="s">
+        <v>46</v>
+      </c>
+      <c r="S5">
+        <v>2932</v>
+      </c>
+      <c r="T5">
+        <v>29049823</v>
+      </c>
+      <c r="U5" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6">
         <v>100</v>
@@ -818,32 +933,47 @@
         <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" t="s">
-        <v>25</v>
+        <v>32</v>
+      </c>
+      <c r="J6">
+        <v>999238821</v>
       </c>
       <c r="K6">
-        <v>999238821</v>
+        <v>2324981042</v>
       </c>
       <c r="L6">
-        <v>2324981042</v>
-      </c>
-      <c r="M6">
         <f>F6*50%</f>
         <v>50</v>
       </c>
-      <c r="N6" s="5">
+      <c r="M6" s="5">
         <v>44899</v>
       </c>
-      <c r="O6" s="6">
-        <v>50</v>
-      </c>
-      <c r="P6" s="5">
+      <c r="N6" s="6">
+        <v>50</v>
+      </c>
+      <c r="O6" s="5">
         <v>44905</v>
+      </c>
+      <c r="P6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>53</v>
+      </c>
+      <c r="R6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6">
+        <v>2948</v>
+      </c>
+      <c r="T6">
+        <v>29308492</v>
+      </c>
+      <c r="U6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>